<commit_message>
repaired the weighing function
</commit_message>
<xml_diff>
--- a/Data/Batches.xlsx
+++ b/Data/Batches.xlsx
@@ -470,6 +470,216 @@
   </x:si>
   <x:si>
     <x:t>2025-10-29 15:38:13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH026</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-05 11:40:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-07 11:40:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 11:40:50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 11:47:41</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH027</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 11:53:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-05 11:53:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 11:53:30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 12:02:07</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH028</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-04 12:02:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-06 12:02:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 12:02:25</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 12:15:33</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH029</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-04 12:21:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-14 12:21:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 12:21:27</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 12:25:24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH030</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 12:30:17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 12:31:51</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH031</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 12:36:48</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 12:38:17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH032</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 13:57:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 13:58:27</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH033</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:01:37</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:02:45</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH034</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:06:23</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:07:27</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH035</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:10:43</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:11:26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH036</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:15:40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:16:48</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH037</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:28:12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:29:24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH038</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:36:18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:37:37</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH039</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:39:53</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:40:43</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH040</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:42:30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:49:32</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH041</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:49:47</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:51:34</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH042</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:51:28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:52:37</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH043</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:52:33</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:52:47</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH044</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:52:57</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 14:57:14</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH045</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 15:02:33</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH046</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-03 15:02:38</x:t>
+  </x:si>
+  <x:si>
+    <x:t>InProgress</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -2225,6 +2435,1119 @@
         <x:v>19</x:v>
       </x:c>
     </x:row>
+    <x:row r="27" spans="1:17">
+      <x:c r="A27" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>145</x:v>
+      </x:c>
+      <x:c r="D27" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E27" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F27" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G27" s="0" t="s">
+        <x:v>153</x:v>
+      </x:c>
+      <x:c r="H27" s="0" t="s">
+        <x:v>154</x:v>
+      </x:c>
+      <x:c r="I27" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J27" s="2">
+        <x:v>45964.4866810764</x:v>
+      </x:c>
+      <x:c r="K27" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L27" s="0" t="s">
+        <x:v>155</x:v>
+      </x:c>
+      <x:c r="M27" s="0" t="s">
+        <x:v>156</x:v>
+      </x:c>
+      <x:c r="N27" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="O27" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="P27" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="Q27" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:17">
+      <x:c r="A28" s="0" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>145</x:v>
+      </x:c>
+      <x:c r="D28" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E28" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F28" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G28" s="0" t="s">
+        <x:v>158</x:v>
+      </x:c>
+      <x:c r="H28" s="0" t="s">
+        <x:v>159</x:v>
+      </x:c>
+      <x:c r="I28" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J28" s="2">
+        <x:v>45964.4954732986</x:v>
+      </x:c>
+      <x:c r="K28" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L28" s="0" t="s">
+        <x:v>160</x:v>
+      </x:c>
+      <x:c r="M28" s="0" t="s">
+        <x:v>161</x:v>
+      </x:c>
+      <x:c r="N28" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="O28" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="P28" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="Q28" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:17">
+      <x:c r="A29" s="0" t="s">
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>145</x:v>
+      </x:c>
+      <x:c r="D29" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E29" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F29" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G29" s="0" t="s">
+        <x:v>163</x:v>
+      </x:c>
+      <x:c r="H29" s="0" t="s">
+        <x:v>164</x:v>
+      </x:c>
+      <x:c r="I29" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J29" s="2">
+        <x:v>45964.5016708218</x:v>
+      </x:c>
+      <x:c r="K29" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L29" s="0" t="s">
+        <x:v>165</x:v>
+      </x:c>
+      <x:c r="M29" s="0" t="s">
+        <x:v>166</x:v>
+      </x:c>
+      <x:c r="N29" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="O29" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="P29" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="Q29" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:17">
+      <x:c r="A30" s="0" t="s">
+        <x:v>167</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="D30" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E30" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F30" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G30" s="0" t="s">
+        <x:v>168</x:v>
+      </x:c>
+      <x:c r="H30" s="0" t="s">
+        <x:v>169</x:v>
+      </x:c>
+      <x:c r="I30" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J30" s="2">
+        <x:v>45964.5148892014</x:v>
+      </x:c>
+      <x:c r="K30" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L30" s="0" t="s">
+        <x:v>170</x:v>
+      </x:c>
+      <x:c r="M30" s="0" t="s">
+        <x:v>171</x:v>
+      </x:c>
+      <x:c r="N30" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="O30" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="P30" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="Q30" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:17">
+      <x:c r="A31" s="0" t="s">
+        <x:v>172</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="D31" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E31" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F31" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G31" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H31" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I31" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J31" s="2">
+        <x:v>45964.5210120486</x:v>
+      </x:c>
+      <x:c r="K31" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L31" s="0" t="s">
+        <x:v>173</x:v>
+      </x:c>
+      <x:c r="M31" s="0" t="s">
+        <x:v>174</x:v>
+      </x:c>
+      <x:c r="N31" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="O31" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="P31" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="Q31" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:17">
+      <x:c r="A32" s="0" t="s">
+        <x:v>175</x:v>
+      </x:c>
+      <x:c r="B32" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="D32" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E32" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F32" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G32" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H32" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I32" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J32" s="2">
+        <x:v>45964.525545625</x:v>
+      </x:c>
+      <x:c r="K32" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L32" s="0" t="s">
+        <x:v>176</x:v>
+      </x:c>
+      <x:c r="M32" s="0" t="s">
+        <x:v>177</x:v>
+      </x:c>
+      <x:c r="N32" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="O32" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="P32" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="Q32" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:17">
+      <x:c r="A33" s="0" t="s">
+        <x:v>178</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="D33" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E33" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F33" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G33" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H33" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I33" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J33" s="2">
+        <x:v>45964.5812575694</x:v>
+      </x:c>
+      <x:c r="K33" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L33" s="0" t="s">
+        <x:v>179</x:v>
+      </x:c>
+      <x:c r="M33" s="0" t="s">
+        <x:v>180</x:v>
+      </x:c>
+      <x:c r="N33" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="O33" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="P33" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="Q33" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:17">
+      <x:c r="A34" s="0" t="s">
+        <x:v>181</x:v>
+      </x:c>
+      <x:c r="B34" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="D34" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E34" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F34" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G34" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H34" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I34" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J34" s="2">
+        <x:v>45964.5844427662</x:v>
+      </x:c>
+      <x:c r="K34" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L34" s="0" t="s">
+        <x:v>182</x:v>
+      </x:c>
+      <x:c r="M34" s="0" t="s">
+        <x:v>183</x:v>
+      </x:c>
+      <x:c r="N34" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="O34" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="P34" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="Q34" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:17">
+      <x:c r="A35" s="0" t="s">
+        <x:v>184</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="D35" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E35" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F35" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G35" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H35" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I35" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J35" s="2">
+        <x:v>45964.5877541898</x:v>
+      </x:c>
+      <x:c r="K35" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L35" s="0" t="s">
+        <x:v>185</x:v>
+      </x:c>
+      <x:c r="M35" s="0" t="s">
+        <x:v>186</x:v>
+      </x:c>
+      <x:c r="N35" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="O35" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="P35" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="Q35" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:17">
+      <x:c r="A36" s="0" t="s">
+        <x:v>187</x:v>
+      </x:c>
+      <x:c r="B36" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="D36" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E36" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F36" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G36" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H36" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I36" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J36" s="2">
+        <x:v>45964.5907683565</x:v>
+      </x:c>
+      <x:c r="K36" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L36" s="0" t="s">
+        <x:v>188</x:v>
+      </x:c>
+      <x:c r="M36" s="0" t="s">
+        <x:v>189</x:v>
+      </x:c>
+      <x:c r="N36" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="O36" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="P36" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="Q36" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:17">
+      <x:c r="A37" s="0" t="s">
+        <x:v>190</x:v>
+      </x:c>
+      <x:c r="B37" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C37" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="D37" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E37" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F37" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G37" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H37" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I37" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J37" s="2">
+        <x:v>45964.5941959144</x:v>
+      </x:c>
+      <x:c r="K37" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L37" s="0" t="s">
+        <x:v>191</x:v>
+      </x:c>
+      <x:c r="M37" s="0" t="s">
+        <x:v>192</x:v>
+      </x:c>
+      <x:c r="N37" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="O37" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="P37" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="Q37" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:17">
+      <x:c r="A38" s="0" t="s">
+        <x:v>193</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C38" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="D38" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E38" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F38" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G38" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H38" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I38" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J38" s="2">
+        <x:v>45964.6029051968</x:v>
+      </x:c>
+      <x:c r="K38" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L38" s="0" t="s">
+        <x:v>194</x:v>
+      </x:c>
+      <x:c r="M38" s="0" t="s">
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="N38" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="O38" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="P38" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="Q38" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:17">
+      <x:c r="A39" s="0" t="s">
+        <x:v>196</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C39" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="D39" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E39" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F39" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G39" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H39" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I39" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J39" s="2">
+        <x:v>45964.6085346065</x:v>
+      </x:c>
+      <x:c r="K39" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L39" s="0" t="s">
+        <x:v>197</x:v>
+      </x:c>
+      <x:c r="M39" s="0" t="s">
+        <x:v>198</x:v>
+      </x:c>
+      <x:c r="N39" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="O39" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="P39" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="Q39" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:17">
+      <x:c r="A40" s="0" t="s">
+        <x:v>199</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C40" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="D40" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E40" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F40" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G40" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H40" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I40" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J40" s="2">
+        <x:v>45964.6110165857</x:v>
+      </x:c>
+      <x:c r="K40" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L40" s="0" t="s">
+        <x:v>200</x:v>
+      </x:c>
+      <x:c r="M40" s="0" t="s">
+        <x:v>201</x:v>
+      </x:c>
+      <x:c r="N40" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="O40" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="P40" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="Q40" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:17">
+      <x:c r="A41" s="0" t="s">
+        <x:v>202</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C41" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="D41" s="0">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E41" s="0">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F41" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G41" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H41" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I41" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J41" s="2">
+        <x:v>45964.6128383681</x:v>
+      </x:c>
+      <x:c r="K41" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L41" s="0" t="s">
+        <x:v>203</x:v>
+      </x:c>
+      <x:c r="M41" s="0" t="s">
+        <x:v>204</x:v>
+      </x:c>
+      <x:c r="N41" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="O41" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="P41" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="Q41" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:17">
+      <x:c r="A42" s="0" t="s">
+        <x:v>205</x:v>
+      </x:c>
+      <x:c r="B42" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C42" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="D42" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E42" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F42" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="G42" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H42" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I42" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J42" s="2">
+        <x:v>45964.6178605556</x:v>
+      </x:c>
+      <x:c r="K42" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L42" s="0" t="s">
+        <x:v>206</x:v>
+      </x:c>
+      <x:c r="M42" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="N42" s="0" t="s">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="O42" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="P42" s="0" t="s">
+        <x:v>207</x:v>
+      </x:c>
+      <x:c r="Q42" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:17">
+      <x:c r="A43" s="0" t="s">
+        <x:v>208</x:v>
+      </x:c>
+      <x:c r="B43" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C43" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="D43" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E43" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F43" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="G43" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H43" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I43" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J43" s="2">
+        <x:v>45964.6190658681</x:v>
+      </x:c>
+      <x:c r="K43" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L43" s="0" t="s">
+        <x:v>209</x:v>
+      </x:c>
+      <x:c r="M43" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="N43" s="0" t="s">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="O43" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="P43" s="0" t="s">
+        <x:v>210</x:v>
+      </x:c>
+      <x:c r="Q43" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:17">
+      <x:c r="A44" s="0" t="s">
+        <x:v>211</x:v>
+      </x:c>
+      <x:c r="B44" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C44" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="D44" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E44" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F44" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="G44" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H44" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I44" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J44" s="2">
+        <x:v>45964.6198176852</x:v>
+      </x:c>
+      <x:c r="K44" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L44" s="0" t="s">
+        <x:v>212</x:v>
+      </x:c>
+      <x:c r="M44" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="N44" s="0" t="s">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="O44" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="P44" s="0" t="s">
+        <x:v>213</x:v>
+      </x:c>
+      <x:c r="Q44" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:17">
+      <x:c r="A45" s="0" t="s">
+        <x:v>214</x:v>
+      </x:c>
+      <x:c r="B45" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C45" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="D45" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E45" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F45" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="G45" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H45" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I45" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J45" s="2">
+        <x:v>45964.6200550347</x:v>
+      </x:c>
+      <x:c r="K45" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L45" s="0" t="s">
+        <x:v>215</x:v>
+      </x:c>
+      <x:c r="M45" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="N45" s="0" t="s">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="O45" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="P45" s="0" t="s">
+        <x:v>216</x:v>
+      </x:c>
+      <x:c r="Q45" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:17">
+      <x:c r="A46" s="0" t="s">
+        <x:v>217</x:v>
+      </x:c>
+      <x:c r="B46" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C46" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="D46" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E46" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F46" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="G46" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H46" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I46" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J46" s="2">
+        <x:v>45964.620093912</x:v>
+      </x:c>
+      <x:c r="K46" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L46" s="0" t="s">
+        <x:v>215</x:v>
+      </x:c>
+      <x:c r="M46" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="N46" s="0" t="s">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="O46" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="P46" s="0" t="s">
+        <x:v>218</x:v>
+      </x:c>
+      <x:c r="Q46" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:17">
+      <x:c r="A47" s="0" t="s">
+        <x:v>219</x:v>
+      </x:c>
+      <x:c r="B47" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C47" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="D47" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E47" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F47" s="0" t="s">
+        <x:v>221</x:v>
+      </x:c>
+      <x:c r="G47" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H47" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="I47" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J47" s="2">
+        <x:v>45964.6268204051</x:v>
+      </x:c>
+      <x:c r="K47" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="L47" s="0" t="s">
+        <x:v>220</x:v>
+      </x:c>
+      <x:c r="M47" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="N47" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="O47" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="P47" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="Q47" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
finalize all features of the system
</commit_message>
<xml_diff>
--- a/Data/Batches.xlsx
+++ b/Data/Batches.xlsx
@@ -679,7 +679,43 @@
     <x:t>2025-11-03 15:02:38</x:t>
   </x:si>
   <x:si>
+    <x:t>no need</x:t>
+  </x:si>
+  <x:si>
+    <x:t>adibsv</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-05 11:57:01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH047</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Official - Recipe 01</x:t>
+  </x:si>
+  <x:si>
     <x:t>InProgress</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-06 10:55:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-06 11:55:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-05 11:55:40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BATCH048</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-05 12:10:36</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-06 12:10:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-11-08 12:10:00</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -3512,7 +3548,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="F47" s="0" t="s">
-        <x:v>221</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="G47" s="0" t="s">
         <x:v>19</x:v>
@@ -3536,15 +3572,121 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="N47" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="O47" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="P47" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="Q47" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:17">
+      <x:c r="A48" s="0" t="s">
+        <x:v>224</x:v>
+      </x:c>
+      <x:c r="B48" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C48" s="0" t="s">
+        <x:v>225</x:v>
+      </x:c>
+      <x:c r="D48" s="0">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="E48" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F48" s="0" t="s">
+        <x:v>226</x:v>
+      </x:c>
+      <x:c r="G48" s="0" t="s">
+        <x:v>227</x:v>
+      </x:c>
+      <x:c r="H48" s="0" t="s">
+        <x:v>228</x:v>
+      </x:c>
+      <x:c r="I48" s="0" t="s">
+        <x:v>222</x:v>
+      </x:c>
+      <x:c r="J48" s="2">
+        <x:v>45966.4969015509</x:v>
+      </x:c>
+      <x:c r="K48" s="0" t="s">
+        <x:v>222</x:v>
+      </x:c>
+      <x:c r="L48" s="0" t="s">
+        <x:v>229</x:v>
+      </x:c>
+      <x:c r="M48" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="N48" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="O48" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="P48" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="Q48" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:17">
+      <x:c r="A49" s="0" t="s">
+        <x:v>230</x:v>
+      </x:c>
+      <x:c r="B49" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C49" s="0" t="s">
+        <x:v>225</x:v>
+      </x:c>
+      <x:c r="D49" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E49" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F49" s="0" t="s">
+        <x:v>226</x:v>
+      </x:c>
+      <x:c r="G49" s="0" t="s">
+        <x:v>232</x:v>
+      </x:c>
+      <x:c r="H49" s="0" t="s">
+        <x:v>233</x:v>
+      </x:c>
+      <x:c r="I49" s="0" t="s">
+        <x:v>222</x:v>
+      </x:c>
+      <x:c r="J49" s="2">
+        <x:v>45966.507346088</x:v>
+      </x:c>
+      <x:c r="K49" s="0" t="s">
+        <x:v>222</x:v>
+      </x:c>
+      <x:c r="L49" s="0" t="s">
+        <x:v>231</x:v>
+      </x:c>
+      <x:c r="M49" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="N49" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="O49" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="P49" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="Q49" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
     </x:row>

</xml_diff>